<commit_message>
bob took architechtral style
</commit_message>
<xml_diff>
--- a/ITEMS TO FINISH.xlsx
+++ b/ITEMS TO FINISH.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moata\source\repos\SW2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammed Ehab\Desktop\SW2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6CD4B75-33B8-4457-9A61-1858EEDD3861}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32EB79A5-79DC-4F5D-BC04-78F4BA503E16}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Iteams</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>Cost</t>
+  </si>
+  <si>
+    <t>Ehab</t>
   </si>
 </sst>
 </file>
@@ -429,16 +432,16 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -446,7 +449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -457,7 +460,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -468,7 +471,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -476,7 +479,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -484,7 +487,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -495,7 +498,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -503,15 +506,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -519,7 +525,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -527,7 +533,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -535,7 +541,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -543,7 +549,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
bob took architechtral design
</commit_message>
<xml_diff>
--- a/ITEMS TO FINISH.xlsx
+++ b/ITEMS TO FINISH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammed Ehab\Desktop\SW2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281DEA7E-58EE-4F1A-9756-F8D11F2035F0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF417129-31CE-49F8-89B5-D68D5C6C30AB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Iteams</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Ehab</t>
+  </si>
+  <si>
+    <t>ehab</t>
   </si>
 </sst>
 </file>
@@ -432,7 +435,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -478,6 +481,9 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">

</xml_diff>

<commit_message>
bob took views and viewpoints
</commit_message>
<xml_diff>
--- a/ITEMS TO FINISH.xlsx
+++ b/ITEMS TO FINISH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammed Ehab\Desktop\SW2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA6704A-2DEE-43AA-85C7-6571419729FE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF801E8-ACB0-4EEB-B240-A1D60874EA21}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Iteams</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>Cost</t>
+  </si>
+  <si>
+    <t>Ehab</t>
   </si>
 </sst>
 </file>
@@ -429,7 +432,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -505,6 +508,9 @@
       <c r="B7" t="s">
         <v>9</v>
       </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">

</xml_diff>

<commit_message>
modified to sally's remarks
</commit_message>
<xml_diff>
--- a/ITEMS TO FINISH.xlsx
+++ b/ITEMS TO FINISH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammed Ehab\Desktop\SW2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990A9269-6F20-4F83-BB60-DF78E7867365}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8F0726-527B-458F-B72E-DE8CBACFA455}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -447,13 +447,13 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="31.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>